<commit_message>
Se actualiza repositorio con los contenidos de cierre de la segnda unidad del curso
</commit_message>
<xml_diff>
--- a/src/test/resources/data/DataPruebas.xlsx
+++ b/src/test/resources/data/DataPruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domingo.saavedra\Documents\SeleniumFalabella\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D85194A-B49E-439A-855C-170E20D50CC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90083027-83E5-46F1-A399-1F4A261C6E0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>TituloCPs</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Dato12</t>
   </si>
   <si>
-    <t>CP002</t>
-  </si>
-  <si>
     <t>CP003</t>
   </si>
   <si>
@@ -119,13 +116,22 @@
     <t>CP001_creacion_cta</t>
   </si>
   <si>
-    <t>e458das7678@algo.com</t>
-  </si>
-  <si>
     <t>adasdas12</t>
   </si>
   <si>
     <t>USer Test 001</t>
+  </si>
+  <si>
+    <t>CP002_iniciar_sesion</t>
+  </si>
+  <si>
+    <t>e4587y87678@algo.com</t>
+  </si>
+  <si>
+    <t>Pobre Dgo</t>
+  </si>
+  <si>
+    <t>e4r5dfs432fs8@algo.com</t>
   </si>
 </sst>
 </file>
@@ -149,12 +155,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -170,9 +182,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -481,7 +494,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,7 +505,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -534,16 +547,16 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E2">
         <v>13</v>
@@ -557,107 +570,111 @@
       <c r="H2">
         <v>0</v>
       </c>
+      <c r="I2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{2385CF18-750D-4C4B-98EB-92B8EC74D6B7}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{EB3BB166-90B1-4C7A-8D1C-126D40F0D9CE}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{2385CF18-750D-4C4B-98EB-92B8EC74D6B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Tarea 2 version inicial
</commit_message>
<xml_diff>
--- a/src/test/resources/data/DataPruebas.xlsx
+++ b/src/test/resources/data/DataPruebas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domingo.saavedra\Documents\SeleniumFalabella\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cristian.moraga\IdeaProjects\TrabajoPOM_Moraga\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90083027-83E5-46F1-A399-1F4A261C6E0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E8C2A0-63EC-4B42-9F7E-9FEE081CE27D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>TituloCPs</t>
   </si>
@@ -71,15 +71,6 @@
     <t>Dato12</t>
   </si>
   <si>
-    <t>CP003</t>
-  </si>
-  <si>
-    <t>CP004</t>
-  </si>
-  <si>
-    <t>CP005</t>
-  </si>
-  <si>
     <t>CP006</t>
   </si>
   <si>
@@ -116,22 +107,46 @@
     <t>CP001_creacion_cta</t>
   </si>
   <si>
-    <t>adasdas12</t>
-  </si>
-  <si>
-    <t>USer Test 001</t>
-  </si>
-  <si>
-    <t>CP002_iniciar_sesion</t>
-  </si>
-  <si>
-    <t>e4587y87678@algo.com</t>
-  </si>
-  <si>
-    <t>Pobre Dgo</t>
-  </si>
-  <si>
-    <t>e4r5dfs432fs8@algo.com</t>
+    <t>Cristian</t>
+  </si>
+  <si>
+    <t>Moraga</t>
+  </si>
+  <si>
+    <t>clave123</t>
+  </si>
+  <si>
+    <t>Congratulations! Your new account has been successfully created!</t>
+  </si>
+  <si>
+    <t>correo4@gmail.com</t>
+  </si>
+  <si>
+    <t>CP002_validar_creacion_cuenta_antigua</t>
+  </si>
+  <si>
+    <t>My Account</t>
+  </si>
+  <si>
+    <t>cmoraga.ochoa@gmail.com</t>
+  </si>
+  <si>
+    <t>CP003_validar_login_correcto</t>
+  </si>
+  <si>
+    <t>Warning: E-Mail Address is already registered!</t>
+  </si>
+  <si>
+    <t>CP004_agregar_producto_carro</t>
+  </si>
+  <si>
+    <t>Success: You have added MacBook to your shopping cart!</t>
+  </si>
+  <si>
+    <t>Your order has been placed!</t>
+  </si>
+  <si>
+    <t>CP005_producto_carro_confirm_order</t>
   </si>
 </sst>
 </file>
@@ -471,7 +486,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -483,7 +498,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -494,17 +509,18 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="60.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -545,136 +561,168 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2">
+        <v>977595472</v>
+      </c>
+      <c r="F2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2">
-        <v>13</v>
-      </c>
-      <c r="F2">
-        <v>12</v>
-      </c>
-      <c r="G2">
-        <v>1991</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3">
+        <v>977595472</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4">
+        <v>123456</v>
+      </c>
+      <c r="D4" t="s">
         <v>31</v>
       </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5">
+        <v>123456</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <v>123456</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{EB3BB166-90B1-4C7A-8D1C-126D40F0D9CE}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{2385CF18-750D-4C4B-98EB-92B8EC74D6B7}"/>
+    <hyperlink ref="B2" r:id="rId1" display="e4r5dfs432fs8@algo.com" xr:uid="{2385CF18-750D-4C4B-98EB-92B8EC74D6B7}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{82204D29-227B-4A97-ABAE-54C306B24E93}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{A214A1C2-3472-4AA2-8673-60EEE54BF0EE}"/>
+    <hyperlink ref="B3" r:id="rId4" display="e4r5dfs432fs8@algo.com" xr:uid="{B4EAEB04-1B1D-413D-83DA-AD798FB7C61A}"/>
+    <hyperlink ref="D3" r:id="rId5" xr:uid="{872DE3F7-B472-422D-B3E5-C41205DCCD89}"/>
+    <hyperlink ref="B5" r:id="rId6" xr:uid="{3504AF40-698B-4225-82B4-57C91D18C417}"/>
+    <hyperlink ref="B6" r:id="rId7" xr:uid="{57A5B179-A3F6-456A-8D3F-774EBBBED742}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -684,7 +732,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -696,7 +744,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -708,7 +756,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>